<commit_message>
Data de los usuarios a los que se califico
</commit_message>
<xml_diff>
--- a/datos/datos_recalificar_emparejamiento.xlsx
+++ b/datos/datos_recalificar_emparejamiento.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t xml:space="preserve">CURSOS_ID</t>
   </si>
@@ -32,13 +32,10 @@
     <t xml:space="preserve">ID_PREGUNTA</t>
   </si>
   <si>
-    <t xml:space="preserve">CPS1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T01.01.07,B001,N1[Pregunta de prueba]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CPS1.2</t>
+    <t xml:space="preserve">CPS1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRUEBA_EMPAREJAMIENTO  </t>
   </si>
   <si>
     <t xml:space="preserve">ENUNCIADOS</t>
@@ -47,13 +44,16 @@
     <t xml:space="preserve">RESPUESTAS</t>
   </si>
   <si>
-    <t xml:space="preserve">Esta es una pregunta de emparejamiento</t>
+    <t xml:space="preserve">¿Es 1 + 1 = 2?</t>
   </si>
   <si>
     <t xml:space="preserve">Verdadero</t>
   </si>
   <si>
-    <t xml:space="preserve">Esta es una pregunta calculada</t>
+    <t xml:space="preserve">¿Es 2 + 2 = 4?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Es 1 + 1 = 3?</t>
   </si>
   <si>
     <t xml:space="preserve">Falso</t>
@@ -63,10 +63,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;VERDADERO&quot;;&quot;VERDADERO&quot;;&quot;FALSO&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -106,6 +107,14 @@
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -152,7 +161,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -179,6 +188,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -201,7 +218,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -237,8 +254,8 @@
       <c r="A3" s="3" t="n">
         <v>13317</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>4</v>
@@ -330,10 +347,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -344,35 +361,42 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>